<commit_message>
Added Missile Launcher + Missile object.
</commit_message>
<xml_diff>
--- a/Acrylicor_Feature_List.xlsx
+++ b/Acrylicor_Feature_List.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Acrylica\Dropbox\DigiPen\Acrylicor_GameEngine\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Acrylica\Dropbox\DigiPen\Acrylicor_GameEngine\Acrylicor\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="72">
   <si>
     <t>Frame Rate Controller</t>
   </si>
@@ -235,6 +235,12 @@
   </si>
   <si>
     <t>EventManager.cpp, AcryEvent.cpp, *Event.cpp</t>
+  </si>
+  <si>
+    <t>WeaponComponent.h, MissileLauncherComponent.h</t>
+  </si>
+  <si>
+    <t>WeaponComponent.cpp, MissileLauncherComponent.cpp</t>
   </si>
 </sst>
 </file>
@@ -720,8 +726,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" topLeftCell="C7" workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1079,8 +1085,14 @@
       <c r="A31" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="B31" s="19" t="s">
-        <v>40</v>
+      <c r="B31" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C31" s="17" t="s">
+        <v>70</v>
+      </c>
+      <c r="D31" s="17" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Final push for project submission.
</commit_message>
<xml_diff>
--- a/Acrylicor_Feature_List.xlsx
+++ b/Acrylicor_Feature_List.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18625"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Acrylica\Dropbox\DigiPen\Acrylicor_GameEngine\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Acrylica\Dropbox\DigiPen\Acrylicor_GameEngine\Acrylicor\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="79">
   <si>
     <t>Frame Rate Controller</t>
   </si>
@@ -147,9 +147,6 @@
     <t>No crashes or locks</t>
   </si>
   <si>
-    <t>WIP</t>
-  </si>
-  <si>
     <t>TransformComponent.h</t>
   </si>
   <si>
@@ -262,6 +259,9 @@
   </si>
   <si>
     <t>WeaponComponent.cpp, MissileLauncherComponent.cpp</t>
+  </si>
+  <si>
+    <t>Boy do I hope so!</t>
   </si>
 </sst>
 </file>
@@ -748,7 +748,7 @@
   <dimension ref="A1:D39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -788,58 +788,58 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B3" s="21" t="s">
         <v>6</v>
       </c>
       <c r="C3" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="D3" s="18" t="s">
         <v>52</v>
-      </c>
-      <c r="D3" s="18" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="22" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>6</v>
       </c>
       <c r="C4" s="22" t="s">
+        <v>67</v>
+      </c>
+      <c r="D4" s="18" t="s">
         <v>68</v>
-      </c>
-      <c r="D4" s="18" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="B5" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="B5" s="21" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="18" t="s">
+      <c r="D5" s="18" t="s">
         <v>50</v>
-      </c>
-      <c r="D5" s="18" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="B6" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="B6" s="21" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" s="18" t="s">
-        <v>45</v>
-      </c>
       <c r="D6" s="18" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -914,10 +914,10 @@
         <v>6</v>
       </c>
       <c r="C13" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="D13" s="17" t="s">
         <v>46</v>
-      </c>
-      <c r="D13" s="17" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -928,10 +928,10 @@
         <v>6</v>
       </c>
       <c r="C14" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="D14" s="17" t="s">
         <v>41</v>
-      </c>
-      <c r="D14" s="17" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -942,10 +942,10 @@
         <v>6</v>
       </c>
       <c r="C15" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="D15" s="17" t="s">
         <v>54</v>
-      </c>
-      <c r="D15" s="17" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -990,24 +990,24 @@
         <v>6</v>
       </c>
       <c r="C20" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="D20" s="17" t="s">
         <v>58</v>
-      </c>
-      <c r="D20" s="17" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="24" t="s">
+        <v>56</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C21" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="B21" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C21" s="17" t="s">
+      <c r="D21" s="17" t="s">
         <v>58</v>
-      </c>
-      <c r="D21" s="17" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -1018,15 +1018,15 @@
         <v>6</v>
       </c>
       <c r="C22" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="D22" s="17" t="s">
         <v>60</v>
-      </c>
-      <c r="D22" s="17" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="23" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B23" s="13" t="s">
         <v>20</v>
@@ -1066,10 +1066,10 @@
         <v>6</v>
       </c>
       <c r="C27" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="D27" s="17" t="s">
         <v>62</v>
-      </c>
-      <c r="D27" s="17" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -1088,7 +1088,7 @@
         <v>6</v>
       </c>
       <c r="C29" s="17" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -1099,10 +1099,10 @@
         <v>6</v>
       </c>
       <c r="C30" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="D30" s="17" t="s">
         <v>64</v>
-      </c>
-      <c r="D30" s="17" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -1113,10 +1113,10 @@
         <v>6</v>
       </c>
       <c r="C31" s="17" t="s">
+        <v>70</v>
+      </c>
+      <c r="D31" s="17" t="s">
         <v>71</v>
-      </c>
-      <c r="D31" s="17" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -1127,10 +1127,10 @@
         <v>6</v>
       </c>
       <c r="C32" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="D32" s="17" t="s">
         <v>77</v>
-      </c>
-      <c r="D32" s="17" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -1141,26 +1141,26 @@
         <v>6</v>
       </c>
       <c r="C33" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="D33" s="17" t="s">
         <v>66</v>
-      </c>
-      <c r="D33" s="17" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="B34" s="13" t="s">
-        <v>20</v>
+      <c r="B34" s="7" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="B35" s="19" t="s">
-        <v>40</v>
+      <c r="B35" s="7" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -1171,10 +1171,10 @@
         <v>6</v>
       </c>
       <c r="C36" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="D36" s="17" t="s">
         <v>73</v>
-      </c>
-      <c r="D36" s="17" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -1184,6 +1184,9 @@
       <c r="B37" s="13" t="s">
         <v>20</v>
       </c>
+      <c r="C37" s="17" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="12" t="s">
@@ -1193,10 +1196,10 @@
         <v>6</v>
       </c>
       <c r="C38" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="D38" s="17" t="s">
         <v>75</v>
-      </c>
-      <c r="D38" s="17" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>